<commit_message>
new version of env/model with 16 groups
</commit_message>
<xml_diff>
--- a/data/jane_model_data/ScenarioPlanFranceOne.xlsx
+++ b/data/jane_model_data/ScenarioPlanFranceOne.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28060" windowHeight="12180" firstSheet="4" activeTab="7"/>
+    <workbookView windowWidth="28800" windowHeight="11560" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="resultsPlots" sheetId="18" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168">
   <si>
     <t>Results Plots (resultsPlotsPHACII)</t>
   </si>
@@ -471,6 +471,21 @@
     <t>Coverage threshold</t>
   </si>
   <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.8</t>
+  </si>
+  <si>
+    <t>0.9</t>
+  </si>
+  <si>
+    <t>0.95</t>
+  </si>
+  <si>
     <t>Efficacy (rho)</t>
   </si>
   <si>
@@ -530,15 +545,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="0.00000"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.0000"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0000"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="178" formatCode="0.00000"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,16 +621,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -628,39 +636,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -674,8 +658,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -690,8 +675,54 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -706,30 +737,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -742,7 +750,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -811,7 +819,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -823,169 +945,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1026,24 +992,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1055,6 +1003,45 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1094,172 +1081,151 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1306,7 +1272,7 @@
     <xf numFmtId="58" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -1320,7 +1286,7 @@
     <xf numFmtId="58" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -1328,10 +1294,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="40"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="178" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="8" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -8141,14 +8107,14 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="vacsi_fra_2021_03_31_10h03" displayName="vacsi_fra_2021_03_31_10h03" ref="A1:H94" totalsRowShown="0">
   <autoFilter ref="A1:H94"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="fra" uniqueName="1" queryTableFieldId="1"/>
-    <tableColumn id="2" name="jour" uniqueName="2" queryTableFieldId="2"/>
-    <tableColumn id="3" name="n_dose1" uniqueName="3" queryTableFieldId="3"/>
-    <tableColumn id="4" name="n_dose2" uniqueName="4" queryTableFieldId="4"/>
-    <tableColumn id="5" name="n_cum_dose1" uniqueName="5" queryTableFieldId="5"/>
-    <tableColumn id="6" name="couv_dose1" uniqueName="6" queryTableFieldId="6"/>
-    <tableColumn id="7" name="n_cum_dose2" uniqueName="7" queryTableFieldId="7"/>
-    <tableColumn id="8" name="couv_dose2" uniqueName="8" queryTableFieldId="8"/>
+    <tableColumn id="1" name="fra"/>
+    <tableColumn id="2" name="jour"/>
+    <tableColumn id="3" name="n_dose1"/>
+    <tableColumn id="4" name="n_dose2"/>
+    <tableColumn id="5" name="n_cum_dose1"/>
+    <tableColumn id="6" name="couv_dose1"/>
+    <tableColumn id="7" name="n_cum_dose2"/>
+    <tableColumn id="8" name="couv_dose2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10794,7 +10760,7 @@
   <sheetPr/>
   <dimension ref="A1:Q78"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="D68" sqref="D68:E78"/>
     </sheetView>
   </sheetViews>
@@ -13704,11 +13670,14 @@
   <sheetPr/>
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -13722,8 +13691,8 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>145</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -13733,8 +13702,8 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
+      <c r="B3" t="s">
+        <v>145</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -13744,8 +13713,8 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>145</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -13755,8 +13724,8 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>0</v>
+      <c r="B5" t="s">
+        <v>145</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -13766,8 +13735,8 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0.7</v>
+      <c r="B6" t="s">
+        <v>146</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -13777,8 +13746,8 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>0.7</v>
+      <c r="B7" t="s">
+        <v>146</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -13788,8 +13757,8 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>0.7</v>
+      <c r="B8" t="s">
+        <v>146</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -13799,8 +13768,8 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0.7</v>
+      <c r="B9" t="s">
+        <v>146</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -13810,8 +13779,8 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>0.7</v>
+      <c r="B10" t="s">
+        <v>146</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -13821,8 +13790,8 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>0.7</v>
+      <c r="B11" t="s">
+        <v>147</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -13832,8 +13801,8 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>0.8</v>
+      <c r="B12" t="s">
+        <v>147</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -13843,8 +13812,8 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>0.8</v>
+      <c r="B13" t="s">
+        <v>147</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -13854,8 +13823,8 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>0.8</v>
+      <c r="B14" t="s">
+        <v>147</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -13865,8 +13834,8 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15">
-        <v>0.8</v>
+      <c r="B15" t="s">
+        <v>148</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -13876,8 +13845,8 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16">
-        <v>0.8</v>
+      <c r="B16" t="s">
+        <v>148</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -13887,8 +13856,8 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>0.8</v>
+      <c r="B17" t="s">
+        <v>149</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -13916,12 +13885,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -13960,7 +13929,7 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -13985,12 +13954,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -14036,7 +14005,7 @@
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="9" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -14062,17 +14031,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -14132,7 +14101,7 @@
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="9" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -14361,7 +14330,7 @@
   <sheetPr/>
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A30" workbookViewId="0">
       <selection activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
@@ -14375,22 +14344,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="B1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="E1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="F1" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="G1" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -14398,7 +14367,7 @@
         <v>43831</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D2" s="1">
         <v>0</v>
@@ -14412,7 +14381,7 @@
         <v>43902</v>
       </c>
       <c r="B3" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D3" s="1">
         <v>0</v>
@@ -14426,7 +14395,7 @@
         <v>43904</v>
       </c>
       <c r="B4" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -14440,7 +14409,7 @@
         <v>43907</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D5" s="1">
         <v>0</v>
@@ -14454,7 +14423,7 @@
         <v>43922</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D6" s="1">
         <v>0</v>
@@ -14468,7 +14437,7 @@
         <v>43952</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D7" s="1">
         <v>0</v>
@@ -14482,7 +14451,7 @@
         <v>43983</v>
       </c>
       <c r="B8" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D8" s="1">
         <v>0</v>
@@ -14496,7 +14465,7 @@
         <v>43984</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D9" s="1">
         <v>0</v>
@@ -14510,7 +14479,7 @@
         <v>44004</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D10" s="1">
         <v>0</v>
@@ -14524,7 +14493,7 @@
         <v>44013</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D11" s="1">
         <v>0</v>
@@ -14538,7 +14507,7 @@
         <v>44016</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -14552,7 +14521,7 @@
         <v>44032</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D13" s="1">
         <v>0</v>
@@ -14566,7 +14535,7 @@
         <v>44044</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
@@ -14580,7 +14549,7 @@
         <v>44070</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
@@ -14594,7 +14563,7 @@
         <v>44075</v>
       </c>
       <c r="B16" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D16" s="1">
         <v>0</v>
@@ -14608,7 +14577,7 @@
         <v>44105</v>
       </c>
       <c r="B17" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -14622,7 +14591,7 @@
         <v>44121</v>
       </c>
       <c r="B18" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D18" s="1">
         <v>0</v>
@@ -14637,7 +14606,7 @@
         <v>44126</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
@@ -14652,7 +14621,7 @@
         <v>44134</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D20" s="1">
         <v>0</v>
@@ -14667,7 +14636,7 @@
         <v>44136</v>
       </c>
       <c r="B21" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D21" s="1">
         <v>0</v>
@@ -14682,7 +14651,7 @@
         <v>44166</v>
       </c>
       <c r="B22" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D22" s="1">
         <v>0</v>
@@ -14697,7 +14666,7 @@
         <v>44180</v>
       </c>
       <c r="B23" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D23" s="1">
         <v>0</v>
@@ -14712,7 +14681,7 @@
         <v>44184</v>
       </c>
       <c r="B24" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D24" s="1">
         <v>0</v>
@@ -14734,7 +14703,7 @@
         <v>44197</v>
       </c>
       <c r="B25" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D25" s="1">
         <f>$E$26*$F25+$B$27</f>
@@ -14757,7 +14726,7 @@
         <v>44200</v>
       </c>
       <c r="B26" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D26" s="1">
         <f>$E$26*$F26+$B$27</f>
@@ -14783,7 +14752,7 @@
         <v>3.3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D27" s="4">
         <f>E27*F27+$B$27</f>
@@ -14806,7 +14775,7 @@
         <v>44208</v>
       </c>
       <c r="B28" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" ref="D28:D31" si="2">E28*F28+$B$27</f>
@@ -14829,7 +14798,7 @@
         <v>44212</v>
       </c>
       <c r="B29" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="2"/>
@@ -14852,7 +14821,7 @@
         <v>44215</v>
       </c>
       <c r="B30" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="2"/>
@@ -14878,7 +14847,7 @@
         <v>17.5</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="2"/>
@@ -14901,7 +14870,7 @@
         <v>44228</v>
       </c>
       <c r="B32" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="1">
@@ -14925,7 +14894,7 @@
         <v>44229</v>
       </c>
       <c r="B33" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D33" s="1">
         <f>E33*F33+$D$31</f>
@@ -14948,7 +14917,7 @@
         <v>44233</v>
       </c>
       <c r="B34" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" ref="D34:D37" si="4">E34*F34+$D$31</f>
@@ -14971,7 +14940,7 @@
         <v>44235</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="4"/>
@@ -14994,7 +14963,7 @@
         <v>44236</v>
       </c>
       <c r="B36" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="4"/>
@@ -15020,7 +14989,7 @@
         <v>51</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D37" s="4">
         <f t="shared" si="4"/>
@@ -15226,7 +15195,7 @@
         <v>85.7</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D50" s="8">
         <f t="shared" si="7"/>
@@ -15663,7 +15632,7 @@
     </row>
     <row r="81" spans="1:1">
       <c r="A81" s="3" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -18404,8 +18373,8 @@
   <sheetPr/>
   <dimension ref="A1:X39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="$A13:$XFD13"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14"/>
@@ -32417,7 +32386,7 @@
   <sheetPr/>
   <dimension ref="A2:DH93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="W4" sqref="W4:Y80"/>

</xml_diff>